<commit_message>
Fixed errors in Calvert datasheets.
</commit_message>
<xml_diff>
--- a/files/kc10.xlsx
+++ b/files/kc10.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\justin.belluz\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\justin.belluz\Documents\R\microscopy_OBIS\files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{057C8983-8C10-4508-8985-AC10B5771EC6}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8214495F-3465-4BE5-9634-6BA5CDCC6C76}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="30720" windowHeight="13380" activeTab="1" xr2:uid="{72E15C2D-14A2-482D-B460-7992896F2F4E}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="30720" windowHeight="13380" xr2:uid="{72E15C2D-14A2-482D-B460-7992896F2F4E}"/>
   </bookViews>
   <sheets>
     <sheet name="KC10_1" sheetId="1" r:id="rId1"/>
@@ -1276,8 +1276,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{07CDF056-AD76-4B4C-AE8D-3035A214141D}">
   <dimension ref="A1:AA210"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A202" sqref="A200:XFD202"/>
+    <sheetView tabSelected="1" topLeftCell="A175" workbookViewId="0">
+      <selection activeCell="A200" sqref="A200"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -6953,9 +6953,6 @@
       </c>
       <c r="B199" s="1"/>
       <c r="C199" s="3"/>
-      <c r="Y199">
-        <v>361677</v>
-      </c>
     </row>
     <row r="200" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A200" s="2" t="s">
@@ -6963,6 +6960,9 @@
       </c>
       <c r="B200" s="2"/>
       <c r="C200" s="3"/>
+      <c r="Y200">
+        <v>361677</v>
+      </c>
     </row>
     <row r="201" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A201" s="3" t="s">
@@ -7161,8 +7161,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{98CC3F34-06EA-4D32-A0CD-A7778C54ACF4}">
   <dimension ref="A1:G217"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A190" workbookViewId="0">
-      <selection activeCell="B1" sqref="B1:D1048576"/>
+    <sheetView topLeftCell="A190" workbookViewId="0">
+      <selection activeCell="A208" sqref="A208:XFD208"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>